<commit_message>
day14 C01 and C02 are added
</commit_message>
<xml_diff>
--- a/src/test/java/day13_excelOtomasyonu/ulkeler.xlsx
+++ b/src/test/java/day13_excelOtomasyonu/ulkeler.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="577">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1735,6 +1735,18 @@
   </si>
   <si>
     <t>Zimbabve</t>
+  </si>
+  <si>
+    <t>Nufus</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>54000</t>
   </si>
 </sst>
 </file>
@@ -2783,7 +2795,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E18"/>
@@ -2791,7 +2803,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.82857142857143" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="4" width="25.6666666666667" customWidth="1"/>
+    <col min="1" max="4" customWidth="true" width="25.6666666666667"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" spans="1:4">
@@ -2807,6 +2819,9 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>573</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
@@ -2821,6 +2836,9 @@
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s" s="0">
+        <v>574</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
@@ -2933,6 +2951,9 @@
       <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="E10" t="s" s="0">
+        <v>575</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
@@ -3002,6 +3023,9 @@
       </c>
       <c r="D15" s="6" t="s">
         <v>49</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>576</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5487,66 +5511,66 @@
   <sheetFormatPr defaultColWidth="8.82857142857143" defaultRowHeight="15" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4">
+      <c r="B4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8">
+      <c r="B8" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="4:4">
-      <c r="D9">
+      <c r="D9" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="3:5">
-      <c r="C12">
+      <c r="C12" s="0">
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15">
+      <c r="B15" s="0">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>11</v>
       </c>
     </row>

</xml_diff>